<commit_message>
✨ feat(analisis): Regenerar archivos Excel con estadísticas detalladas para mejorar el análisis y la claridad de los resultados.
</commit_message>
<xml_diff>
--- a/analisis/01_PASO1_NORMALIDAD_SHAPIRO_WILK.xlsx
+++ b/analisis/01_PASO1_NORMALIDAD_SHAPIRO_WILK.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Shapiro_N12" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Shapiro_N2480" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Shapiro_N12" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -483,6 +484,368 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Instruction Coverage (%)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.816008043429448</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.337136908350902e-39</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>19.941</v>
+      </c>
+      <c r="I2" t="n">
+        <v>12.1149437230795</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Instruction Coverage (%)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>880</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.7523643876549621</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.663606854482367e-34</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>14.20104545454545</v>
+      </c>
+      <c r="I3" t="n">
+        <v>8.707367967776438</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Branch Coverage (%)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1600</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.8177699142698152</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.214917981583953e-39</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>17.6875</v>
+      </c>
+      <c r="I4" t="n">
+        <v>12.39259674296598</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Branch Coverage (%)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>880</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8697179827556469</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.968664763323198e-26</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>13.50284090909091</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6.747887032681644</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mutation Score (%)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1600</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8404116629778383</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.458931328321721e-37</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>22.918</v>
+      </c>
+      <c r="I6" t="n">
+        <v>17.1925242563866</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mutation Score (%)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>880</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8313344102201263</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.820920203199541e-29</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>16.63388636363636</v>
+      </c>
+      <c r="I7" t="n">
+        <v>8.160557021954679</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Time (seconds)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1600</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.479676697019995</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8.07180512008333e-56</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0.079395625</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1775453021479479</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>N=2,480</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Time (seconds)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>880</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5354067631882183</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.671058967064643e-43</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0.1140261363636364</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.231760935630358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nivel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Metrica</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Grupo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>W_statistic</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Es_Normal</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Desv_Est</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>N=12</t>
         </is>
       </c>

</xml_diff>